<commit_message>
added model for Lithuania
</commit_message>
<xml_diff>
--- a/data/AW_raw_data.xlsx
+++ b/data/AW_raw_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vogelwarte-my.sharepoint.com/personal/steffen_oppel_vogelwarte_ch/Documents/AQWA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vogelwarte-my.sharepoint.com/personal/steffen_oppel_vogelwarte_ch/Documents/AQWA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_91688F0743E7EABA05502068677980F108A5B899" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D334876-A6C6-4400-B24E-FCB5095C5CBB}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_91688F0743E7EABA05502068677980F108A5B899" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{863EF870-0CD8-4419-898A-AC036D9F2FCD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pom.Pop" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="115">
   <si>
     <t>count</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>Nrel</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -765,16 +768,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D32" sqref="D32:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="11.44140625" style="2"/>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>111</v>
@@ -787,7 +790,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1993</v>
       </c>
@@ -803,7 +806,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1994</v>
       </c>
@@ -817,7 +820,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1995</v>
       </c>
@@ -831,7 +834,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1996</v>
       </c>
@@ -845,7 +848,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1997</v>
       </c>
@@ -861,7 +864,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1998</v>
       </c>
@@ -875,7 +878,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1999</v>
       </c>
@@ -889,7 +892,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2000</v>
       </c>
@@ -903,7 +906,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2001</v>
       </c>
@@ -917,7 +920,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2002</v>
       </c>
@@ -931,7 +934,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2003</v>
       </c>
@@ -947,7 +950,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2004</v>
       </c>
@@ -963,7 +966,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2005</v>
       </c>
@@ -979,7 +982,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2006</v>
       </c>
@@ -995,7 +998,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2007</v>
       </c>
@@ -1011,7 +1014,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2008</v>
       </c>
@@ -1027,7 +1030,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2009</v>
       </c>
@@ -1043,7 +1046,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2010</v>
       </c>
@@ -1059,7 +1062,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2011</v>
       </c>
@@ -1075,7 +1078,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2012</v>
       </c>
@@ -1091,7 +1094,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2013</v>
       </c>
@@ -1107,7 +1110,7 @@
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2014</v>
       </c>
@@ -1123,7 +1126,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2015</v>
       </c>
@@ -1139,7 +1142,7 @@
       </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2016</v>
       </c>
@@ -1155,7 +1158,7 @@
       </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2017</v>
       </c>
@@ -1171,7 +1174,7 @@
       </c>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2018</v>
       </c>
@@ -1187,7 +1190,7 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2019</v>
       </c>
@@ -1203,7 +1206,7 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2020</v>
       </c>
@@ -1219,7 +1222,7 @@
       </c>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2021</v>
       </c>
@@ -1235,7 +1238,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2022</v>
       </c>
@@ -1251,7 +1254,7 @@
       </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -1271,7 +1274,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2024</v>
       </c>
@@ -1291,21 +1294,21 @@
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1321,20 +1324,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1993</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1994</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1995</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1996</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1997</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1998</v>
       </c>
@@ -1382,7 +1388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1999</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2000</v>
       </c>
@@ -1398,7 +1404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2001</v>
       </c>
@@ -1406,7 +1412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2003</v>
       </c>
@@ -1422,7 +1428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2004</v>
       </c>
@@ -1430,7 +1436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2005</v>
       </c>
@@ -1438,7 +1444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2006</v>
       </c>
@@ -1446,7 +1452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2007</v>
       </c>
@@ -1454,7 +1460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2008</v>
       </c>
@@ -1462,7 +1468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2009</v>
       </c>
@@ -1470,7 +1476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2010</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -1486,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2012</v>
       </c>
@@ -1494,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2013</v>
       </c>
@@ -1502,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2014</v>
       </c>
@@ -1510,7 +1516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2015</v>
       </c>
@@ -1518,7 +1524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2016</v>
       </c>
@@ -1526,7 +1532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2017</v>
       </c>
@@ -1534,7 +1540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>2018</v>
       </c>
@@ -1546,7 +1552,7 @@
       </c>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>2019</v>
       </c>
@@ -1558,7 +1564,7 @@
       </c>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2020</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2021</v>
       </c>
@@ -1574,7 +1580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2022</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2023</v>
       </c>
@@ -1590,9 +1596,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2024</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2025</v>
       </c>
     </row>
   </sheetData>
@@ -1609,13 +1620,13 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1650,7 +1661,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1676,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1702,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1728,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1754,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1780,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1806,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1832,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1858,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1884,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1910,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1936,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1962,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1988,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2014,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2040,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -2066,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -2092,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2118,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2144,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2170,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2196,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2222,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2248,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -2274,7 +2285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2300,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2326,7 +2337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -2352,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2378,7 +2389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2404,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -2430,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -2456,7 +2467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -2482,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -2508,7 +2519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2534,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -2560,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -2586,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -2612,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2638,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -2664,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -2690,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2716,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2742,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -2768,7 +2779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -2794,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2820,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2846,7 +2857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -2872,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -2898,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -2924,7 +2935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2950,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2976,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -3002,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>75</v>
       </c>
@@ -3028,7 +3039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -3054,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -3080,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -3106,7 +3117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>83</v>
       </c>
@@ -3132,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -3158,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -3184,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -3210,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -3236,7 +3247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>87</v>
       </c>
@@ -3262,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -3288,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -3314,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -3340,7 +3351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>59</v>
       </c>
@@ -3366,7 +3377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -3392,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -3418,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -3444,7 +3455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>55</v>
       </c>
@@ -3470,7 +3481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -3496,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -3522,7 +3533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>94</v>
       </c>
@@ -3548,7 +3559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>95</v>
       </c>
@@ -3574,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>54</v>
       </c>
@@ -3600,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>57</v>
       </c>
@@ -3626,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -3652,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -3678,7 +3689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>67</v>
       </c>
@@ -3704,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>68</v>
       </c>
@@ -3730,7 +3741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>76</v>
       </c>
@@ -3756,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -3782,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -3808,7 +3819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>69</v>
       </c>
@@ -3834,7 +3845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>70</v>
       </c>
@@ -3860,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>77</v>
       </c>
@@ -3886,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>92</v>
       </c>
@@ -3912,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>93</v>
       </c>
@@ -3938,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>56</v>
       </c>
@@ -3964,7 +3975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -3990,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>97</v>
       </c>
@@ -4016,7 +4027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>98</v>
       </c>
@@ -4042,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -4068,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>73</v>
       </c>
@@ -4094,7 +4105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>74</v>
       </c>
@@ -4120,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -4146,7 +4157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -4172,7 +4183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -4198,7 +4209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>103</v>
       </c>

</xml_diff>